<commit_message>
Updates for Version 2.0 in documentation
</commit_message>
<xml_diff>
--- a/Documenation/0000-VersioningTables.xlsx
+++ b/Documenation/0000-VersioningTables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anzij\Source\Repos\CustomerAdministration\Documenation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Clouds\OwnCloud\FH\6_Semester\ASW6IL\Project\Repos\CustomerAdministration\Documenation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32F45CE-8E88-4852-AC7E-3F4CD51254E0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60CA62F-1628-424E-8490-E6961AEF8AD3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3743" activeTab="1" xr2:uid="{116BF198-297D-4556-B4BB-F9479836182F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3743" firstSheet="1" activeTab="3" xr2:uid="{116BF198-297D-4556-B4BB-F9479836182F}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>Projcect No.</t>
   </si>
@@ -66,6 +66,9 @@
     <t>JoAn
 MiVu
 WiLe</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
 </sst>
 </file>
@@ -257,10 +260,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -584,13 +587,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.75">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
@@ -620,13 +623,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069E1B54-68AA-4C90-AEA9-ACD1A8C32A6D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -654,12 +657,11 @@
       <c r="B2" s="3">
         <v>1000</v>
       </c>
-      <c r="C2" s="3" t="str">
-        <f>General!B4</f>
-        <v>1.0</v>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="4">
-        <v>43230</v>
+        <v>43241</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>11</v>
@@ -679,7 +681,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -712,12 +714,11 @@
       <c r="B2" s="3">
         <v>2000</v>
       </c>
-      <c r="C2" s="3" t="str">
-        <f>General!B4</f>
-        <v>1.0</v>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="4">
-        <v>43230</v>
+        <v>43241</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>11</v>
@@ -736,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76E3BC2-215D-4DE3-9A7A-3615A5281BBE}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -770,12 +771,11 @@
       <c r="B2" s="3">
         <v>9000</v>
       </c>
-      <c r="C2" s="3" t="str">
-        <f>General!B4</f>
-        <v>1.0</v>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="4">
-        <v>43230</v>
+        <v>43241</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>11</v>

</xml_diff>